<commit_message>
Queue Send Email ke Semua Petugas
</commit_message>
<xml_diff>
--- a/public/dummy/petugas_peralatan.xlsx
+++ b/public/dummy/petugas_peralatan.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EAS PBO\verynewest\Sistem_Peminjaman_Peralatan\public\dummy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEKOLAH\KULIAH\SEMESTER 3\PEMROGRAMAN_BERORIENTASI_OBJEK\Sistem_Peminjaman_Peralatan\public\dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBE6AA3-4F92-40BC-8E54-B9522FB84F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E41D8C5-CB93-4D0A-A581-3AD9F1C9C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Adam Siswanto</t>
   </si>
@@ -119,13 +132,46 @@
   </si>
   <si>
     <t>budi123</t>
+  </si>
+  <si>
+    <t>budi99@gmail.com</t>
+  </si>
+  <si>
+    <t>setiawan99@gmail.com</t>
+  </si>
+  <si>
+    <t>yannuardy99@gmail.com</t>
+  </si>
+  <si>
+    <t>adam99@gmail.com</t>
+  </si>
+  <si>
+    <t>sumantri99@gmail.com</t>
+  </si>
+  <si>
+    <t>farhan99@gmail.com</t>
+  </si>
+  <si>
+    <t>nathasya99@gmail.com</t>
+  </si>
+  <si>
+    <t>nurjaman99@gmail.com</t>
+  </si>
+  <si>
+    <t>hilmi99@gmail.com</t>
+  </si>
+  <si>
+    <t>andre99@gmail.com</t>
+  </si>
+  <si>
+    <t>joko99@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -152,11 +198,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -177,7 +223,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -476,10 +522,10 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="4" width="14.85546875" customWidth="1"/>
@@ -487,7 +533,7 @@
     <col min="6" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -497,8 +543,11 @@
       <c r="C1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -508,11 +557,13 @@
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -522,11 +573,13 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,11 +589,13 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -550,11 +605,13 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -564,11 +621,13 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -578,11 +637,13 @@
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -592,11 +653,13 @@
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -606,11 +669,13 @@
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -620,11 +685,13 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -634,7 +701,9 @@
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>

</xml_diff>

<commit_message>
FIX: Activity Log, MPDF, dan UI
</commit_message>
<xml_diff>
--- a/public/dummy/petugas_peralatan.xlsx
+++ b/public/dummy/petugas_peralatan.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEKOLAH\KULIAH\SEMESTER 3\PEMROGRAMAN_BERORIENTASI_OBJEK\Sistem_Peminjaman_Peralatan\public\dummy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EAS PBO\verynewest\Equipment\public\dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E41D8C5-CB93-4D0A-A581-3AD9F1C9C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F8FCA7B-9235-44B4-8A93-D9B3DD2CC1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C7082C4-D1EB-4083-AD1C-7EEF6C76CFBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -24,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,138 +34,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+  <si>
+    <t>Budi</t>
+  </si>
+  <si>
+    <t>budi99</t>
+  </si>
+  <si>
+    <t>budi123</t>
+  </si>
+  <si>
+    <t>budi99@gmail.com</t>
+  </si>
+  <si>
+    <t>Setiawan</t>
+  </si>
+  <si>
+    <t>setiawan99</t>
+  </si>
+  <si>
+    <t>setiawan123</t>
+  </si>
+  <si>
+    <t>setiawan99@gmail.com</t>
+  </si>
+  <si>
+    <t>Yannuardy</t>
+  </si>
+  <si>
+    <t>yannuardy99</t>
+  </si>
+  <si>
+    <t>yannuardy123</t>
+  </si>
+  <si>
+    <t>yannuardy99@gmail.com</t>
+  </si>
   <si>
     <t>Adam Siswanto</t>
   </si>
   <si>
-    <t>Yannuardy</t>
-  </si>
-  <si>
-    <t>Setiawan</t>
+    <t>adam99</t>
+  </si>
+  <si>
+    <t>adam123</t>
+  </si>
+  <si>
+    <t>adam99@gmail.com</t>
   </si>
   <si>
     <t>Sumantri</t>
   </si>
   <si>
+    <t>sumantri99</t>
+  </si>
+  <si>
+    <t>sumantri123</t>
+  </si>
+  <si>
+    <t>sumantri99@gmail.com</t>
+  </si>
+  <si>
     <t>Farhan</t>
   </si>
   <si>
+    <t>farhan99</t>
+  </si>
+  <si>
+    <t>farhan123</t>
+  </si>
+  <si>
+    <t>farhan99@gmail.com</t>
+  </si>
+  <si>
     <t>Nathasya</t>
   </si>
   <si>
+    <t>nathasya99</t>
+  </si>
+  <si>
+    <t>nathasya123</t>
+  </si>
+  <si>
+    <t>nathasya99@gmail.com</t>
+  </si>
+  <si>
     <t>Nurjaman</t>
   </si>
   <si>
+    <t>nurjaman99</t>
+  </si>
+  <si>
+    <t>nurjaman123</t>
+  </si>
+  <si>
+    <t>nurjaman99@gmail.com</t>
+  </si>
+  <si>
     <t>Hilmi</t>
   </si>
   <si>
+    <t>hilmi99</t>
+  </si>
+  <si>
+    <t>hilmi123</t>
+  </si>
+  <si>
+    <t>hilmi99@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andre </t>
   </si>
   <si>
+    <t>andre99</t>
+  </si>
+  <si>
+    <t>andre123</t>
+  </si>
+  <si>
+    <t>andre99@gmail.com</t>
+  </si>
+  <si>
     <t>Joko</t>
   </si>
   <si>
-    <t>adam123</t>
-  </si>
-  <si>
-    <t>yannuardy123</t>
-  </si>
-  <si>
-    <t>setiawan123</t>
-  </si>
-  <si>
-    <t>sumantri123</t>
-  </si>
-  <si>
-    <t>farhan123</t>
-  </si>
-  <si>
-    <t>nathasya123</t>
-  </si>
-  <si>
-    <t>nurjaman123</t>
-  </si>
-  <si>
-    <t>hilmi123</t>
-  </si>
-  <si>
-    <t>andre123</t>
+    <t>joko99</t>
   </si>
   <si>
     <t>joko123</t>
   </si>
   <si>
-    <t>adam99</t>
-  </si>
-  <si>
-    <t>yannuardy99</t>
-  </si>
-  <si>
-    <t>setiawan99</t>
-  </si>
-  <si>
-    <t>sumantri99</t>
-  </si>
-  <si>
-    <t>farhan99</t>
-  </si>
-  <si>
-    <t>nathasya99</t>
-  </si>
-  <si>
-    <t>nurjaman99</t>
-  </si>
-  <si>
-    <t>hilmi99</t>
-  </si>
-  <si>
-    <t>andre99</t>
-  </si>
-  <si>
-    <t>joko99</t>
-  </si>
-  <si>
-    <t>budi</t>
-  </si>
-  <si>
-    <t>budi99</t>
-  </si>
-  <si>
-    <t>budi123</t>
-  </si>
-  <si>
-    <t>budi99@gmail.com</t>
-  </si>
-  <si>
-    <t>setiawan99@gmail.com</t>
-  </si>
-  <si>
-    <t>yannuardy99@gmail.com</t>
-  </si>
-  <si>
-    <t>adam99@gmail.com</t>
-  </si>
-  <si>
-    <t>sumantri99@gmail.com</t>
-  </si>
-  <si>
-    <t>farhan99@gmail.com</t>
-  </si>
-  <si>
-    <t>nathasya99@gmail.com</t>
-  </si>
-  <si>
-    <t>nurjaman99@gmail.com</t>
-  </si>
-  <si>
-    <t>hilmi99@gmail.com</t>
-  </si>
-  <si>
-    <t>andre99@gmail.com</t>
-  </si>
-  <si>
     <t>joko99@gmail.com</t>
+  </si>
+  <si>
+    <t>Kohjad</t>
+  </si>
+  <si>
+    <t>Kokoh12</t>
+  </si>
+  <si>
+    <t>12Kokoh</t>
+  </si>
+  <si>
+    <t>Kokoh12@gmail.com</t>
+  </si>
+  <si>
+    <t>Hilda</t>
+  </si>
+  <si>
+    <t>Hilda15</t>
+  </si>
+  <si>
+    <t>1234Hilda</t>
+  </si>
+  <si>
+    <t>Hilda15@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -174,7 +199,10 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,20 +225,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -223,7 +245,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -518,194 +540,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EEFD90-C675-4BE7-BE74-EF50256CD4D2}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>